<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758122676750_backup@backdoor.com.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758122676750_backup@backdoor.com.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758122676750_backup@backdoor.com.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\Imported_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2178B08C-4448-48DF-87C5-1338287616FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AE1F1B-F3AC-4B59-BDD6-283E8A573C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -309,12 +309,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -340,10 +347,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,16 +694,16 @@
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D2" sqref="D2:D85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -715,7 +723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -725,8 +733,8 @@
       <c r="C2" s="1">
         <v>45910</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D2" s="3">
+        <v>0.46059027777777778</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -735,7 +743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -745,8 +753,8 @@
       <c r="C3" s="1">
         <v>45910</v>
       </c>
-      <c r="D3" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D3" s="3">
+        <v>0.46059027777777778</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -755,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -765,8 +773,8 @@
       <c r="C4" s="1">
         <v>45910</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D4" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -775,7 +783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -785,8 +793,8 @@
       <c r="C5" s="1">
         <v>45910</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D5" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -795,7 +803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -805,8 +813,8 @@
       <c r="C6" s="1">
         <v>45910</v>
       </c>
-      <c r="D6" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D6" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -815,7 +823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -825,8 +833,8 @@
       <c r="C7" s="1">
         <v>45910</v>
       </c>
-      <c r="D7" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D7" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
@@ -835,7 +843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -845,8 +853,8 @@
       <c r="C8" s="1">
         <v>45910</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D8" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -855,7 +863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -865,8 +873,8 @@
       <c r="C9" s="1">
         <v>45910</v>
       </c>
-      <c r="D9" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D9" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -875,7 +883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -885,8 +893,8 @@
       <c r="C10" s="1">
         <v>45910</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D10" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -895,7 +903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -905,8 +913,8 @@
       <c r="C11" s="1">
         <v>45910</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D11" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -915,7 +923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -925,8 +933,8 @@
       <c r="C12" s="1">
         <v>45910</v>
       </c>
-      <c r="D12" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D12" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -935,7 +943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -945,8 +953,8 @@
       <c r="C13" s="1">
         <v>45910</v>
       </c>
-      <c r="D13" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D13" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -955,7 +963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -965,8 +973,8 @@
       <c r="C14" s="1">
         <v>45910</v>
       </c>
-      <c r="D14" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D14" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -975,7 +983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -985,8 +993,8 @@
       <c r="C15" s="1">
         <v>45910</v>
       </c>
-      <c r="D15" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D15" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -995,7 +1003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1005,8 +1013,8 @@
       <c r="C16" s="1">
         <v>45910</v>
       </c>
-      <c r="D16" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D16" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
@@ -1015,7 +1023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1025,8 +1033,8 @@
       <c r="C17" s="1">
         <v>45910</v>
       </c>
-      <c r="D17" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D17" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -1035,7 +1043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1045,8 +1053,8 @@
       <c r="C18" s="1">
         <v>45910</v>
       </c>
-      <c r="D18" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D18" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1055,7 +1063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1065,8 +1073,8 @@
       <c r="C19" s="1">
         <v>45910</v>
       </c>
-      <c r="D19" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D19" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1075,7 +1083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1085,8 +1093,8 @@
       <c r="C20" s="1">
         <v>45910</v>
       </c>
-      <c r="D20" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D20" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
@@ -1095,7 +1103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1105,8 +1113,8 @@
       <c r="C21" s="1">
         <v>45910</v>
       </c>
-      <c r="D21" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D21" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1115,7 +1123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1125,8 +1133,8 @@
       <c r="C22" s="1">
         <v>45910</v>
       </c>
-      <c r="D22" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D22" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1135,7 +1143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1145,8 +1153,8 @@
       <c r="C23" s="1">
         <v>45910</v>
       </c>
-      <c r="D23" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D23" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1155,7 +1163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1165,8 +1173,8 @@
       <c r="C24" s="1">
         <v>45910</v>
       </c>
-      <c r="D24" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D24" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1175,7 +1183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1185,8 +1193,8 @@
       <c r="C25" s="1">
         <v>45910</v>
       </c>
-      <c r="D25" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D25" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1195,7 +1203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1205,8 +1213,8 @@
       <c r="C26" s="1">
         <v>45910</v>
       </c>
-      <c r="D26" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D26" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -1215,7 +1223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1225,8 +1233,8 @@
       <c r="C27" s="1">
         <v>45910</v>
       </c>
-      <c r="D27" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D27" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1235,7 +1243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1245,8 +1253,8 @@
       <c r="C28" s="1">
         <v>45910</v>
       </c>
-      <c r="D28" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D28" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
@@ -1255,7 +1263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1265,8 +1273,8 @@
       <c r="C29" s="1">
         <v>45910</v>
       </c>
-      <c r="D29" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D29" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1275,7 +1283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1285,8 +1293,8 @@
       <c r="C30" s="1">
         <v>45910</v>
       </c>
-      <c r="D30" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D30" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -1295,7 +1303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1305,8 +1313,8 @@
       <c r="C31" s="1">
         <v>45910</v>
       </c>
-      <c r="D31" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D31" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
@@ -1315,7 +1323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -1325,8 +1333,8 @@
       <c r="C32" s="1">
         <v>45910</v>
       </c>
-      <c r="D32" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D32" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
@@ -1335,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1345,8 +1353,8 @@
       <c r="C33" s="1">
         <v>45910</v>
       </c>
-      <c r="D33" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D33" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -1355,7 +1363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1365,8 +1373,8 @@
       <c r="C34" s="1">
         <v>45910</v>
       </c>
-      <c r="D34" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D34" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -1375,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1385,8 +1393,8 @@
       <c r="C35" s="1">
         <v>45910</v>
       </c>
-      <c r="D35" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D35" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1395,7 +1403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1405,8 +1413,8 @@
       <c r="C36" s="1">
         <v>45910</v>
       </c>
-      <c r="D36" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D36" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
@@ -1415,7 +1423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1425,8 +1433,8 @@
       <c r="C37" s="1">
         <v>45910</v>
       </c>
-      <c r="D37" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D37" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
@@ -1435,7 +1443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1445,8 +1453,8 @@
       <c r="C38" s="1">
         <v>45910</v>
       </c>
-      <c r="D38" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D38" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
@@ -1455,7 +1463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1465,8 +1473,8 @@
       <c r="C39" s="1">
         <v>45910</v>
       </c>
-      <c r="D39" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D39" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
@@ -1475,7 +1483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1485,8 +1493,8 @@
       <c r="C40" s="1">
         <v>45910</v>
       </c>
-      <c r="D40" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D40" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
@@ -1495,7 +1503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1505,8 +1513,8 @@
       <c r="C41" s="1">
         <v>45910</v>
       </c>
-      <c r="D41" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D41" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
@@ -1515,7 +1523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1525,8 +1533,8 @@
       <c r="C42" s="1">
         <v>45910</v>
       </c>
-      <c r="D42" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D42" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E42" t="s">
         <v>8</v>
@@ -1535,7 +1543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -1545,8 +1553,8 @@
       <c r="C43" s="1">
         <v>45910</v>
       </c>
-      <c r="D43" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D43" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
@@ -1555,7 +1563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1565,8 +1573,8 @@
       <c r="C44" s="1">
         <v>45910</v>
       </c>
-      <c r="D44" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D44" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
@@ -1575,7 +1583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -1585,8 +1593,8 @@
       <c r="C45" s="1">
         <v>45910</v>
       </c>
-      <c r="D45" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D45" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
@@ -1595,7 +1603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -1605,8 +1613,8 @@
       <c r="C46" s="1">
         <v>45910</v>
       </c>
-      <c r="D46" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D46" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
@@ -1615,7 +1623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1625,8 +1633,8 @@
       <c r="C47" s="1">
         <v>45910</v>
       </c>
-      <c r="D47" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D47" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
@@ -1635,7 +1643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1645,8 +1653,8 @@
       <c r="C48" s="1">
         <v>45910</v>
       </c>
-      <c r="D48" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D48" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
@@ -1655,7 +1663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1665,8 +1673,8 @@
       <c r="C49" s="1">
         <v>45910</v>
       </c>
-      <c r="D49" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D49" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
@@ -1675,7 +1683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1685,8 +1693,8 @@
       <c r="C50" s="1">
         <v>45910</v>
       </c>
-      <c r="D50" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D50" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E50" t="s">
         <v>8</v>
@@ -1695,7 +1703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1705,8 +1713,8 @@
       <c r="C51" s="1">
         <v>45910</v>
       </c>
-      <c r="D51" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D51" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E51" t="s">
         <v>8</v>
@@ -1715,7 +1723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1725,8 +1733,8 @@
       <c r="C52" s="1">
         <v>45910</v>
       </c>
-      <c r="D52" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D52" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E52" t="s">
         <v>8</v>
@@ -1735,7 +1743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -1745,8 +1753,8 @@
       <c r="C53" s="1">
         <v>45910</v>
       </c>
-      <c r="D53" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D53" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E53" t="s">
         <v>8</v>
@@ -1755,7 +1763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -1765,8 +1773,8 @@
       <c r="C54" s="1">
         <v>45910</v>
       </c>
-      <c r="D54" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D54" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E54" t="s">
         <v>8</v>
@@ -1775,7 +1783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -1785,8 +1793,8 @@
       <c r="C55" s="1">
         <v>45910</v>
       </c>
-      <c r="D55" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D55" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E55" t="s">
         <v>8</v>
@@ -1795,7 +1803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1805,8 +1813,8 @@
       <c r="C56" s="1">
         <v>45910</v>
       </c>
-      <c r="D56" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D56" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E56" t="s">
         <v>8</v>
@@ -1815,7 +1823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -1825,8 +1833,8 @@
       <c r="C57" s="1">
         <v>45910</v>
       </c>
-      <c r="D57" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D57" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E57" t="s">
         <v>8</v>
@@ -1835,7 +1843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -1845,8 +1853,8 @@
       <c r="C58" s="1">
         <v>45910</v>
       </c>
-      <c r="D58" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D58" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -1855,7 +1863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -1865,8 +1873,8 @@
       <c r="C59" s="1">
         <v>45910</v>
       </c>
-      <c r="D59" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D59" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E59" t="s">
         <v>8</v>
@@ -1875,7 +1883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -1885,8 +1893,8 @@
       <c r="C60" s="1">
         <v>45910</v>
       </c>
-      <c r="D60" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D60" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
@@ -1895,7 +1903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -1905,8 +1913,8 @@
       <c r="C61" s="1">
         <v>45910</v>
       </c>
-      <c r="D61" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D61" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E61" t="s">
         <v>8</v>
@@ -1915,7 +1923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -1925,8 +1933,8 @@
       <c r="C62" s="1">
         <v>45910</v>
       </c>
-      <c r="D62" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D62" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E62" t="s">
         <v>8</v>
@@ -1935,7 +1943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -1945,8 +1953,8 @@
       <c r="C63" s="1">
         <v>45910</v>
       </c>
-      <c r="D63" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D63" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
@@ -1955,7 +1963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -1965,8 +1973,8 @@
       <c r="C64" s="1">
         <v>45910</v>
       </c>
-      <c r="D64" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D64" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E64" t="s">
         <v>15</v>
@@ -1975,7 +1983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -1985,8 +1993,8 @@
       <c r="C65" s="1">
         <v>45910</v>
       </c>
-      <c r="D65" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D65" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -1995,7 +2003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -2005,8 +2013,8 @@
       <c r="C66" s="1">
         <v>45910</v>
       </c>
-      <c r="D66" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D66" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E66" t="s">
         <v>8</v>
@@ -2015,7 +2023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -2025,8 +2033,8 @@
       <c r="C67" s="1">
         <v>45910</v>
       </c>
-      <c r="D67" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D67" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E67" t="s">
         <v>8</v>
@@ -2035,7 +2043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -2045,8 +2053,8 @@
       <c r="C68" s="1">
         <v>45910</v>
       </c>
-      <c r="D68" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D68" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E68" t="s">
         <v>8</v>
@@ -2055,7 +2063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -2065,8 +2073,8 @@
       <c r="C69" s="1">
         <v>45910</v>
       </c>
-      <c r="D69" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D69" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E69" t="s">
         <v>8</v>
@@ -2075,7 +2083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -2085,8 +2093,8 @@
       <c r="C70" s="1">
         <v>45910</v>
       </c>
-      <c r="D70" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D70" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E70" t="s">
         <v>8</v>
@@ -2095,7 +2103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -2105,8 +2113,8 @@
       <c r="C71" s="1">
         <v>45910</v>
       </c>
-      <c r="D71" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D71" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E71" t="s">
         <v>8</v>
@@ -2115,7 +2123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -2125,8 +2133,8 @@
       <c r="C72" s="1">
         <v>45910</v>
       </c>
-      <c r="D72" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D72" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2135,7 +2143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -2145,8 +2153,8 @@
       <c r="C73" s="1">
         <v>45910</v>
       </c>
-      <c r="D73" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D73" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
@@ -2155,7 +2163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -2165,8 +2173,8 @@
       <c r="C74" s="1">
         <v>45910</v>
       </c>
-      <c r="D74" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D74" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E74" t="s">
         <v>8</v>
@@ -2175,7 +2183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -2185,8 +2193,8 @@
       <c r="C75" s="1">
         <v>45910</v>
       </c>
-      <c r="D75" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D75" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E75" t="s">
         <v>8</v>
@@ -2195,7 +2203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -2205,8 +2213,8 @@
       <c r="C76" s="1">
         <v>45910</v>
       </c>
-      <c r="D76" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D76" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
@@ -2215,7 +2223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -2225,8 +2233,8 @@
       <c r="C77" s="1">
         <v>45910</v>
       </c>
-      <c r="D77" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D77" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E77" t="s">
         <v>8</v>
@@ -2235,7 +2243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -2245,8 +2253,8 @@
       <c r="C78" s="1">
         <v>45910</v>
       </c>
-      <c r="D78" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D78" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E78" t="s">
         <v>8</v>
@@ -2255,7 +2263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -2265,8 +2273,8 @@
       <c r="C79" s="1">
         <v>45910</v>
       </c>
-      <c r="D79" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D79" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E79" t="s">
         <v>15</v>
@@ -2275,7 +2283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -2285,8 +2293,8 @@
       <c r="C80" s="1">
         <v>45910</v>
       </c>
-      <c r="D80" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D80" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E80" t="s">
         <v>8</v>
@@ -2295,7 +2303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -2305,8 +2313,8 @@
       <c r="C81" s="1">
         <v>45910</v>
       </c>
-      <c r="D81" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D81" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E81" t="s">
         <v>8</v>
@@ -2315,7 +2323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -2325,8 +2333,8 @@
       <c r="C82" s="1">
         <v>45910</v>
       </c>
-      <c r="D82" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D82" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E82" t="s">
         <v>8</v>
@@ -2335,7 +2343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -2345,8 +2353,8 @@
       <c r="C83" s="1">
         <v>45910</v>
       </c>
-      <c r="D83" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D83" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E83" t="s">
         <v>8</v>
@@ -2355,7 +2363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -2365,8 +2373,8 @@
       <c r="C84" s="1">
         <v>45910</v>
       </c>
-      <c r="D84" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D84" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -2375,7 +2383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -2385,8 +2393,8 @@
       <c r="C85" s="1">
         <v>45910</v>
       </c>
-      <c r="D85" s="2">
-        <v>0.47560185185185183</v>
+      <c r="D85" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>

</xml_diff>